<commit_message>
Update Algo-problem mapping excel
</commit_message>
<xml_diff>
--- a/Algo-Problem mapping.xlsx
+++ b/Algo-Problem mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I524764\Documents\Projects\Data Structures &amp; Algorithms\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35313070-A592-4948-B6B9-BD43D026613F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A6F9F2-00D8-4888-9D53-02D13ACC5FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="364" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Data Structure</t>
   </si>
@@ -64,13 +64,52 @@
   </si>
   <si>
     <t>Loop the array, currentSum += arr[i], maxSum=max(maxSum,currentSum), if currentSum&lt;0 then currentSum=0, return maxSum</t>
+  </si>
+  <si>
+    <t>Quick Sort: Normal, Randomized</t>
+  </si>
+  <si>
+    <t>Flip Bits</t>
+  </si>
+  <si>
+    <t>Given array of integers ARR[] of size N consisting of zeros and ones. Select a subset and flip bits of that subset. Return the count of maximum one’s that you can obtain by flipping chosen sub-array at most once.</t>
+  </si>
+  <si>
+    <t>Loop the array, conver all 1's into -1 and convert all 0's into 1 (Also count total 1's). Now find the max. subarray sum. Return the oneCount + maxSum</t>
+  </si>
+  <si>
+    <t>https://github.com/RAVIGANESHMBHAT/Data-Structures-and-Algorithms/blob/master/2.%20Arrays/1.%20Kadane's%20Algorithm</t>
+  </si>
+  <si>
+    <t>https://github.com/RAVIGANESHMBHAT/Data-Structures-and-Algorithms/blob/master/2.%20Arrays/2.%20Flip%20Bits</t>
+  </si>
+  <si>
+    <t>Maximum Subarray Sum after k concatenation</t>
+  </si>
+  <si>
+    <t>Iterate through original array and find total sum. If k=1, just apply Kadan's algo for the array. If sum &lt;0, apply Kadan's algo for two array concatenated{array.concat(array)}. If  sum &gt;0, then return the Kadan's maxSum for two concatenated arrays + (k-2)*sum</t>
+  </si>
+  <si>
+    <t>Maximum Sum Rectangle</t>
+  </si>
+  <si>
+    <t>Dutch National Flag Algo / Three Way Partitioning Algo</t>
+  </si>
+  <si>
+    <t>Sort array of 0s 1s and 2s in an array</t>
+  </si>
+  <si>
+    <t>Given an array consisting of only 0s, 1s and 2s, sort the array.</t>
+  </si>
+  <si>
+    <t>low=0, mid=0, high=n-1. While mid&lt;=high , if a[mid]==0 then swap(arr[low],arr[mid]) mid++ low++,  if a[mid]==1 then mid++,  if a[mid]==2 then swap(arr[mid],arr[high]) high--</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,13 +133,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -112,16 +163,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -401,20 +455,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.81640625" customWidth="1"/>
     <col min="2" max="2" width="18.7265625" customWidth="1"/>
-    <col min="3" max="3" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.6328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="93" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="93" customWidth="1"/>
-    <col min="6" max="6" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="126.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="111.36328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="46" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -457,15 +511,66 @@
       <c r="E2" t="s">
         <v>12</v>
       </c>
+      <c r="F2" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="G2" s="2" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C5" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E28" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{26A9A4A7-8ED2-4E79-A30D-4D1321D0CCFA}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{16D060B0-EFD8-4FAC-93E8-1F469EDEB81F}"/>
+    <hyperlink ref="F3" r:id="rId3" xr:uid="{AA6C36A4-ED80-41C7-AAA6-2C068A451577}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>